<commit_message>
Fixing bugs, adding log features, saving query results
</commit_message>
<xml_diff>
--- a/Example/AR1 - Q1.2023.xlsx
+++ b/Example/AR1 - Q1.2023.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Krzysztof kaniewski\PycharmProjects\pythonProject\Example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D082979-8A7D-45C1-9138-69DACF2C7D8C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16460125-C46C-4016-966E-1AB70C5B04A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="830" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="830" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ST.01" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="5">ST.06!$B$1:$I$46</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="6">ST.07!$A$1:$J$29</definedName>
   </definedNames>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -2712,7 +2712,7 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="199">
+  <cellXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3083,15 +3083,6 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3251,6 +3242,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -4083,13 +4077,13 @@
       <c r="A7" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="154" t="s">
         <v>47</v>
       </c>
       <c r="C7" s="74" t="s">
         <v>361</v>
       </c>
-      <c r="D7" s="160" t="s">
+      <c r="D7" s="157" t="s">
         <v>179</v>
       </c>
       <c r="E7" s="69" t="s">
@@ -4102,11 +4096,11 @@
       <c r="A8" s="72" t="s">
         <v>78</v>
       </c>
-      <c r="B8" s="158"/>
+      <c r="B8" s="155"/>
       <c r="C8" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="D8" s="160"/>
+      <c r="D8" s="157"/>
       <c r="E8" s="69" t="s">
         <v>363</v>
       </c>
@@ -4117,11 +4111,11 @@
       <c r="A9" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="B9" s="158"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="D9" s="160"/>
+      <c r="D9" s="157"/>
       <c r="E9" s="69" t="s">
         <v>364</v>
       </c>
@@ -4132,11 +4126,11 @@
       <c r="A10" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="B10" s="158"/>
+      <c r="B10" s="155"/>
       <c r="C10" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="160"/>
+      <c r="D10" s="157"/>
       <c r="E10" s="69" t="s">
         <v>50</v>
       </c>
@@ -4147,11 +4141,11 @@
       <c r="A11" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="B11" s="159"/>
+      <c r="B11" s="156"/>
       <c r="C11" s="74" t="s">
         <v>383</v>
       </c>
-      <c r="D11" s="160"/>
+      <c r="D11" s="157"/>
       <c r="E11" s="69" t="s">
         <v>365</v>
       </c>
@@ -4162,13 +4156,13 @@
       <c r="A12" s="73" t="s">
         <v>71</v>
       </c>
-      <c r="B12" s="161" t="s">
+      <c r="B12" s="158" t="s">
         <v>48</v>
       </c>
       <c r="C12" s="74" t="s">
         <v>362</v>
       </c>
-      <c r="D12" s="160" t="s">
+      <c r="D12" s="157" t="s">
         <v>180</v>
       </c>
       <c r="E12" s="69" t="s">
@@ -4181,11 +4175,11 @@
       <c r="A13" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="161"/>
+      <c r="B13" s="158"/>
       <c r="C13" s="74" t="s">
         <v>373</v>
       </c>
-      <c r="D13" s="160"/>
+      <c r="D13" s="157"/>
       <c r="E13" s="69" t="s">
         <v>363</v>
       </c>
@@ -4196,11 +4190,11 @@
       <c r="A14" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="B14" s="161"/>
+      <c r="B14" s="158"/>
       <c r="C14" s="74" t="s">
         <v>374</v>
       </c>
-      <c r="D14" s="160"/>
+      <c r="D14" s="157"/>
       <c r="E14" s="69" t="s">
         <v>364</v>
       </c>
@@ -4211,11 +4205,11 @@
       <c r="A15" s="73" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="161"/>
+      <c r="B15" s="158"/>
       <c r="C15" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="160"/>
+      <c r="D15" s="157"/>
       <c r="E15" s="69" t="s">
         <v>50</v>
       </c>
@@ -4226,13 +4220,13 @@
       <c r="A16" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="B16" s="162" t="s">
+      <c r="B16" s="159" t="s">
         <v>49</v>
       </c>
       <c r="C16" s="74" t="s">
         <v>366</v>
       </c>
-      <c r="D16" s="160" t="s">
+      <c r="D16" s="157" t="s">
         <v>181</v>
       </c>
       <c r="E16" s="69" t="s">
@@ -4245,11 +4239,11 @@
       <c r="A17" s="72" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="162"/>
+      <c r="B17" s="159"/>
       <c r="C17" s="74" t="s">
         <v>375</v>
       </c>
-      <c r="D17" s="160"/>
+      <c r="D17" s="157"/>
       <c r="E17" s="69" t="s">
         <v>367</v>
       </c>
@@ -4260,11 +4254,11 @@
       <c r="A18" s="72" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="162"/>
+      <c r="B18" s="159"/>
       <c r="C18" s="74" t="s">
         <v>376</v>
       </c>
-      <c r="D18" s="160"/>
+      <c r="D18" s="157"/>
       <c r="E18" s="69" t="s">
         <v>363</v>
       </c>
@@ -4275,11 +4269,11 @@
       <c r="A19" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="162"/>
+      <c r="B19" s="159"/>
       <c r="C19" s="74" t="s">
         <v>377</v>
       </c>
-      <c r="D19" s="160"/>
+      <c r="D19" s="157"/>
       <c r="E19" s="69" t="s">
         <v>364</v>
       </c>
@@ -4290,11 +4284,11 @@
       <c r="A20" s="72" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="162"/>
+      <c r="B20" s="159"/>
       <c r="C20" s="74" t="s">
         <v>378</v>
       </c>
-      <c r="D20" s="160"/>
+      <c r="D20" s="157"/>
       <c r="E20" s="69" t="s">
         <v>368</v>
       </c>
@@ -4305,11 +4299,11 @@
       <c r="A21" s="72" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="162"/>
+      <c r="B21" s="159"/>
       <c r="C21" s="74" t="s">
         <v>379</v>
       </c>
-      <c r="D21" s="160"/>
+      <c r="D21" s="157"/>
       <c r="E21" s="69" t="s">
         <v>369</v>
       </c>
@@ -4320,11 +4314,11 @@
       <c r="A22" s="72" t="s">
         <v>89</v>
       </c>
-      <c r="B22" s="162"/>
+      <c r="B22" s="159"/>
       <c r="C22" s="74" t="s">
         <v>380</v>
       </c>
-      <c r="D22" s="160"/>
+      <c r="D22" s="157"/>
       <c r="E22" s="69" t="s">
         <v>370</v>
       </c>
@@ -4335,11 +4329,11 @@
       <c r="A23" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="B23" s="162"/>
+      <c r="B23" s="159"/>
       <c r="C23" s="74" t="s">
         <v>381</v>
       </c>
-      <c r="D23" s="160"/>
+      <c r="D23" s="157"/>
       <c r="E23" s="69" t="s">
         <v>371</v>
       </c>
@@ -4350,11 +4344,11 @@
       <c r="A24" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="B24" s="162"/>
+      <c r="B24" s="159"/>
       <c r="C24" s="74" t="s">
         <v>382</v>
       </c>
-      <c r="D24" s="160"/>
+      <c r="D24" s="157"/>
       <c r="E24" s="69" t="s">
         <v>372</v>
       </c>
@@ -4365,11 +4359,11 @@
       <c r="A25" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="162"/>
+      <c r="B25" s="159"/>
       <c r="C25" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="D25" s="160"/>
+      <c r="D25" s="157"/>
       <c r="E25" s="69" t="s">
         <v>176</v>
       </c>
@@ -5043,13 +5037,13 @@
       <c r="A8" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="166" t="s">
+      <c r="B8" s="163" t="s">
         <v>8</v>
       </c>
       <c r="C8" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="168" t="s">
+      <c r="D8" s="165" t="s">
         <v>185</v>
       </c>
       <c r="E8" s="68" t="s">
@@ -5062,11 +5056,11 @@
       <c r="A9" s="48" t="s">
         <v>93</v>
       </c>
-      <c r="B9" s="167"/>
+      <c r="B9" s="164"/>
       <c r="C9" s="54" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="169"/>
+      <c r="D9" s="166"/>
       <c r="E9" s="68" t="s">
         <v>50</v>
       </c>
@@ -5077,7 +5071,7 @@
       <c r="A10" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="163" t="s">
+      <c r="B10" s="160" t="s">
         <v>384</v>
       </c>
       <c r="C10" s="44" t="s">
@@ -5096,7 +5090,7 @@
       <c r="A11" s="46" t="s">
         <v>95</v>
       </c>
-      <c r="B11" s="164"/>
+      <c r="B11" s="161"/>
       <c r="C11" s="61" t="s">
         <v>392</v>
       </c>
@@ -5111,7 +5105,7 @@
       <c r="A12" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="B12" s="164"/>
+      <c r="B12" s="161"/>
       <c r="C12" s="61" t="s">
         <v>388</v>
       </c>
@@ -5126,7 +5120,7 @@
       <c r="A13" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="B13" s="164"/>
+      <c r="B13" s="161"/>
       <c r="C13" s="61" t="s">
         <v>393</v>
       </c>
@@ -5141,7 +5135,7 @@
       <c r="A14" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="B14" s="165"/>
+      <c r="B14" s="162"/>
       <c r="C14" s="55" t="s">
         <v>394</v>
       </c>
@@ -5748,13 +5742,13 @@
       <c r="A8" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="157" t="s">
+      <c r="B8" s="154" t="s">
         <v>47</v>
       </c>
       <c r="C8" s="91" t="s">
         <v>397</v>
       </c>
-      <c r="D8" s="170" t="s">
+      <c r="D8" s="167" t="s">
         <v>179</v>
       </c>
       <c r="E8" s="69" t="s">
@@ -5767,11 +5761,11 @@
       <c r="A9" s="72" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="158"/>
+      <c r="B9" s="155"/>
       <c r="C9" s="91" t="s">
         <v>376</v>
       </c>
-      <c r="D9" s="171"/>
+      <c r="D9" s="168"/>
       <c r="E9" s="69" t="s">
         <v>363</v>
       </c>
@@ -5782,11 +5776,11 @@
       <c r="A10" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="158"/>
+      <c r="B10" s="155"/>
       <c r="C10" s="92" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="171"/>
+      <c r="D10" s="168"/>
       <c r="E10" s="69" t="s">
         <v>50</v>
       </c>
@@ -5797,11 +5791,11 @@
       <c r="A11" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="B11" s="158"/>
+      <c r="B11" s="155"/>
       <c r="C11" s="92" t="s">
         <v>399</v>
       </c>
-      <c r="D11" s="171"/>
+      <c r="D11" s="168"/>
       <c r="E11" s="69" t="s">
         <v>401</v>
       </c>
@@ -5812,11 +5806,11 @@
       <c r="A12" s="72" t="s">
         <v>213</v>
       </c>
-      <c r="B12" s="159"/>
+      <c r="B12" s="156"/>
       <c r="C12" s="91" t="s">
         <v>402</v>
       </c>
-      <c r="D12" s="172"/>
+      <c r="D12" s="169"/>
       <c r="E12" s="69" t="s">
         <v>403</v>
       </c>
@@ -5827,13 +5821,13 @@
       <c r="A13" s="73" t="s">
         <v>104</v>
       </c>
-      <c r="B13" s="157" t="s">
+      <c r="B13" s="154" t="s">
         <v>48</v>
       </c>
       <c r="C13" s="91" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="170" t="s">
+      <c r="D13" s="167" t="s">
         <v>191</v>
       </c>
       <c r="E13" s="69" t="s">
@@ -5846,11 +5840,11 @@
       <c r="A14" s="72" t="s">
         <v>105</v>
       </c>
-      <c r="B14" s="158"/>
+      <c r="B14" s="155"/>
       <c r="C14" s="91" t="s">
         <v>400</v>
       </c>
-      <c r="D14" s="171"/>
+      <c r="D14" s="168"/>
       <c r="E14" s="69" t="s">
         <v>363</v>
       </c>
@@ -5861,11 +5855,11 @@
       <c r="A15" s="73" t="s">
         <v>106</v>
       </c>
-      <c r="B15" s="158"/>
+      <c r="B15" s="155"/>
       <c r="C15" s="92" t="s">
         <v>398</v>
       </c>
-      <c r="D15" s="171"/>
+      <c r="D15" s="168"/>
       <c r="E15" s="69" t="s">
         <v>50</v>
       </c>
@@ -5876,11 +5870,11 @@
       <c r="A16" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="B16" s="159"/>
+      <c r="B16" s="156"/>
       <c r="C16" s="92" t="s">
         <v>399</v>
       </c>
-      <c r="D16" s="172"/>
+      <c r="D16" s="169"/>
       <c r="E16" s="69" t="s">
         <v>401</v>
       </c>
@@ -5891,13 +5885,13 @@
       <c r="A17" s="71" t="s">
         <v>108</v>
       </c>
-      <c r="B17" s="157" t="s">
+      <c r="B17" s="154" t="s">
         <v>49</v>
       </c>
       <c r="C17" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="D17" s="170" t="s">
+      <c r="D17" s="167" t="s">
         <v>192</v>
       </c>
       <c r="E17" s="69" t="s">
@@ -5910,11 +5904,11 @@
       <c r="A18" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="B18" s="159"/>
+      <c r="B18" s="156"/>
       <c r="C18" s="91" t="s">
         <v>400</v>
       </c>
-      <c r="D18" s="172"/>
+      <c r="D18" s="169"/>
       <c r="E18" s="69" t="s">
         <v>363</v>
       </c>
@@ -6449,7 +6443,7 @@
       </c>
       <c r="E6" s="100"/>
       <c r="F6" s="101"/>
-      <c r="G6" s="173" t="s">
+      <c r="G6" s="170" t="s">
         <v>405</v>
       </c>
       <c r="H6" s="103" t="s">
@@ -6469,7 +6463,7 @@
       <c r="F7" s="109" t="s">
         <v>407</v>
       </c>
-      <c r="G7" s="174"/>
+      <c r="G7" s="171"/>
       <c r="H7" s="102"/>
       <c r="I7" s="109" t="s">
         <v>408</v>
@@ -6487,7 +6481,7 @@
       </c>
       <c r="E8" s="105"/>
       <c r="F8" s="106"/>
-      <c r="G8" s="175" t="s">
+      <c r="G8" s="172" t="s">
         <v>199</v>
       </c>
       <c r="H8" s="104" t="s">
@@ -6507,7 +6501,7 @@
       <c r="F9" s="108" t="s">
         <v>411</v>
       </c>
-      <c r="G9" s="176"/>
+      <c r="G9" s="173"/>
       <c r="H9" s="107"/>
       <c r="I9" s="108" t="s">
         <v>390</v>
@@ -7873,18 +7867,18 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-      <c r="J6" s="189" t="s">
+      <c r="J6" s="186" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="189"/>
-      <c r="L6" s="189"/>
-      <c r="M6" s="189"/>
-      <c r="N6" s="189" t="s">
+      <c r="K6" s="186"/>
+      <c r="L6" s="186"/>
+      <c r="M6" s="186"/>
+      <c r="N6" s="186" t="s">
         <v>77</v>
       </c>
-      <c r="O6" s="189"/>
-      <c r="P6" s="189"/>
-      <c r="Q6" s="189"/>
+      <c r="O6" s="186"/>
+      <c r="P6" s="186"/>
+      <c r="Q6" s="186"/>
     </row>
     <row r="7" spans="1:18" s="50" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="56"/>
@@ -7896,22 +7890,22 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-      <c r="J7" s="189" t="s">
+      <c r="J7" s="186" t="s">
         <v>357</v>
       </c>
-      <c r="K7" s="189"/>
-      <c r="L7" s="189" t="s">
+      <c r="K7" s="186"/>
+      <c r="L7" s="186" t="s">
         <v>427</v>
       </c>
-      <c r="M7" s="189"/>
-      <c r="N7" s="189" t="s">
+      <c r="M7" s="186"/>
+      <c r="N7" s="186" t="s">
         <v>428</v>
       </c>
-      <c r="O7" s="189"/>
-      <c r="P7" s="189" t="s">
+      <c r="O7" s="186"/>
+      <c r="P7" s="186" t="s">
         <v>429</v>
       </c>
-      <c r="Q7" s="189"/>
+      <c r="Q7" s="186"/>
     </row>
     <row r="8" spans="1:18" s="50" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A8" s="56"/>
@@ -7958,18 +7952,18 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-      <c r="J9" s="179" t="s">
+      <c r="J9" s="176" t="s">
         <v>204</v>
       </c>
-      <c r="K9" s="179"/>
-      <c r="L9" s="179"/>
-      <c r="M9" s="179"/>
-      <c r="N9" s="179" t="s">
+      <c r="K9" s="176"/>
+      <c r="L9" s="176"/>
+      <c r="M9" s="176"/>
+      <c r="N9" s="176" t="s">
         <v>247</v>
       </c>
-      <c r="O9" s="179"/>
-      <c r="P9" s="179"/>
-      <c r="Q9" s="179"/>
+      <c r="O9" s="176"/>
+      <c r="P9" s="176"/>
+      <c r="Q9" s="176"/>
     </row>
     <row r="10" spans="1:18" s="50" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="56"/>
@@ -7981,22 +7975,22 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-      <c r="J10" s="190" t="s">
+      <c r="J10" s="187" t="s">
         <v>200</v>
       </c>
-      <c r="K10" s="191"/>
-      <c r="L10" s="190" t="s">
+      <c r="K10" s="188"/>
+      <c r="L10" s="187" t="s">
         <v>201</v>
       </c>
-      <c r="M10" s="191"/>
-      <c r="N10" s="179" t="s">
+      <c r="M10" s="188"/>
+      <c r="N10" s="176" t="s">
         <v>251</v>
       </c>
-      <c r="O10" s="179"/>
-      <c r="P10" s="179" t="s">
+      <c r="O10" s="176"/>
+      <c r="P10" s="176" t="s">
         <v>250</v>
       </c>
-      <c r="Q10" s="179"/>
+      <c r="Q10" s="176"/>
     </row>
     <row r="11" spans="1:18" s="50" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A11" s="56"/>
@@ -8037,564 +8031,564 @@
       <c r="A12" s="89" t="s">
         <v>144</v>
       </c>
-      <c r="B12" s="177" t="s">
+      <c r="B12" s="174" t="s">
         <v>252</v>
       </c>
-      <c r="C12" s="178" t="s">
+      <c r="C12" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="178" t="s">
+      <c r="D12" s="175" t="s">
         <v>14</v>
       </c>
       <c r="E12" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="F12" s="179" t="s">
+      <c r="F12" s="176" t="s">
         <v>355</v>
       </c>
-      <c r="G12" s="180" t="s">
+      <c r="G12" s="177" t="s">
         <v>205</v>
       </c>
-      <c r="H12" s="179" t="s">
+      <c r="H12" s="176" t="s">
         <v>207</v>
       </c>
       <c r="I12" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="J12" s="153"/>
-      <c r="K12" s="153"/>
-      <c r="L12" s="154"/>
-      <c r="M12" s="154"/>
-      <c r="N12" s="153"/>
-      <c r="O12" s="153"/>
-      <c r="P12" s="154"/>
-      <c r="Q12" s="154"/>
+      <c r="J12" s="150"/>
+      <c r="K12" s="150"/>
+      <c r="L12" s="151"/>
+      <c r="M12" s="151"/>
+      <c r="N12" s="150"/>
+      <c r="O12" s="150"/>
+      <c r="P12" s="151"/>
+      <c r="Q12" s="151"/>
       <c r="R12" s="43"/>
     </row>
     <row r="13" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="89" t="s">
         <v>158</v>
       </c>
-      <c r="B13" s="177"/>
-      <c r="C13" s="178"/>
-      <c r="D13" s="178"/>
+      <c r="B13" s="174"/>
+      <c r="C13" s="175"/>
+      <c r="D13" s="175"/>
       <c r="E13" s="74" t="s">
         <v>419</v>
       </c>
-      <c r="F13" s="179"/>
-      <c r="G13" s="181"/>
-      <c r="H13" s="179"/>
+      <c r="F13" s="176"/>
+      <c r="G13" s="178"/>
+      <c r="H13" s="176"/>
       <c r="I13" s="84" t="s">
         <v>420</v>
       </c>
-      <c r="J13" s="153"/>
-      <c r="K13" s="153"/>
-      <c r="L13" s="154"/>
-      <c r="M13" s="154"/>
-      <c r="N13" s="153"/>
-      <c r="O13" s="153"/>
-      <c r="P13" s="154"/>
-      <c r="Q13" s="154"/>
+      <c r="J13" s="150"/>
+      <c r="K13" s="150"/>
+      <c r="L13" s="151"/>
+      <c r="M13" s="151"/>
+      <c r="N13" s="150"/>
+      <c r="O13" s="150"/>
+      <c r="P13" s="151"/>
+      <c r="Q13" s="151"/>
       <c r="R13" s="43"/>
     </row>
     <row r="14" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="89" t="s">
         <v>145</v>
       </c>
-      <c r="B14" s="177"/>
-      <c r="C14" s="178"/>
-      <c r="D14" s="178"/>
+      <c r="B14" s="174"/>
+      <c r="C14" s="175"/>
+      <c r="D14" s="175"/>
       <c r="E14" s="117" t="s">
         <v>208</v>
       </c>
-      <c r="F14" s="179"/>
-      <c r="G14" s="181"/>
-      <c r="H14" s="179"/>
+      <c r="F14" s="176"/>
+      <c r="G14" s="178"/>
+      <c r="H14" s="176"/>
       <c r="I14" s="119" t="s">
         <v>208</v>
       </c>
-      <c r="J14" s="153"/>
-      <c r="K14" s="153"/>
-      <c r="L14" s="154"/>
-      <c r="M14" s="154"/>
-      <c r="N14" s="153"/>
-      <c r="O14" s="153"/>
-      <c r="P14" s="154"/>
-      <c r="Q14" s="154"/>
+      <c r="J14" s="150"/>
+      <c r="K14" s="150"/>
+      <c r="L14" s="151"/>
+      <c r="M14" s="151"/>
+      <c r="N14" s="150"/>
+      <c r="O14" s="150"/>
+      <c r="P14" s="151"/>
+      <c r="Q14" s="151"/>
       <c r="R14" s="43"/>
     </row>
     <row r="15" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="89" t="s">
         <v>146</v>
       </c>
-      <c r="B15" s="177"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="178"/>
+      <c r="B15" s="174"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="175"/>
       <c r="E15" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="179"/>
-      <c r="G15" s="181"/>
-      <c r="H15" s="179"/>
+      <c r="F15" s="176"/>
+      <c r="G15" s="178"/>
+      <c r="H15" s="176"/>
       <c r="I15" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="J15" s="153"/>
-      <c r="K15" s="153"/>
-      <c r="L15" s="154"/>
-      <c r="M15" s="154"/>
-      <c r="N15" s="153"/>
-      <c r="O15" s="153"/>
-      <c r="P15" s="154"/>
-      <c r="Q15" s="154"/>
+      <c r="J15" s="150"/>
+      <c r="K15" s="150"/>
+      <c r="L15" s="151"/>
+      <c r="M15" s="151"/>
+      <c r="N15" s="150"/>
+      <c r="O15" s="150"/>
+      <c r="P15" s="151"/>
+      <c r="Q15" s="151"/>
       <c r="R15" s="43"/>
     </row>
     <row r="16" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="89" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="177"/>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178" t="s">
+      <c r="B16" s="174"/>
+      <c r="C16" s="175"/>
+      <c r="D16" s="175" t="s">
         <v>15</v>
       </c>
       <c r="E16" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="179"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="179" t="s">
+      <c r="F16" s="176"/>
+      <c r="G16" s="178"/>
+      <c r="H16" s="176" t="s">
         <v>206</v>
       </c>
       <c r="I16" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="J16" s="153"/>
-      <c r="K16" s="153"/>
-      <c r="L16" s="154"/>
-      <c r="M16" s="154"/>
-      <c r="N16" s="153"/>
-      <c r="O16" s="153"/>
-      <c r="P16" s="154"/>
-      <c r="Q16" s="154"/>
+      <c r="J16" s="150"/>
+      <c r="K16" s="150"/>
+      <c r="L16" s="151"/>
+      <c r="M16" s="151"/>
+      <c r="N16" s="150"/>
+      <c r="O16" s="150"/>
+      <c r="P16" s="151"/>
+      <c r="Q16" s="151"/>
       <c r="R16" s="43"/>
     </row>
     <row r="17" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="89" t="s">
         <v>159</v>
       </c>
-      <c r="B17" s="177"/>
-      <c r="C17" s="178"/>
-      <c r="D17" s="178"/>
+      <c r="B17" s="174"/>
+      <c r="C17" s="175"/>
+      <c r="D17" s="175"/>
       <c r="E17" s="74" t="s">
         <v>419</v>
       </c>
-      <c r="F17" s="179"/>
-      <c r="G17" s="181"/>
-      <c r="H17" s="179"/>
+      <c r="F17" s="176"/>
+      <c r="G17" s="178"/>
+      <c r="H17" s="176"/>
       <c r="I17" s="84" t="s">
         <v>416</v>
       </c>
-      <c r="J17" s="153"/>
-      <c r="K17" s="153"/>
-      <c r="L17" s="154"/>
-      <c r="M17" s="154"/>
-      <c r="N17" s="153"/>
-      <c r="O17" s="153"/>
-      <c r="P17" s="154"/>
-      <c r="Q17" s="154"/>
+      <c r="J17" s="150"/>
+      <c r="K17" s="150"/>
+      <c r="L17" s="151"/>
+      <c r="M17" s="151"/>
+      <c r="N17" s="150"/>
+      <c r="O17" s="150"/>
+      <c r="P17" s="151"/>
+      <c r="Q17" s="151"/>
       <c r="R17" s="43"/>
     </row>
     <row r="18" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="89" t="s">
         <v>148</v>
       </c>
-      <c r="B18" s="177"/>
-      <c r="C18" s="178"/>
-      <c r="D18" s="178"/>
+      <c r="B18" s="174"/>
+      <c r="C18" s="175"/>
+      <c r="D18" s="175"/>
       <c r="E18" s="75" t="s">
         <v>208</v>
       </c>
-      <c r="F18" s="179"/>
-      <c r="G18" s="181"/>
-      <c r="H18" s="179"/>
+      <c r="F18" s="176"/>
+      <c r="G18" s="178"/>
+      <c r="H18" s="176"/>
       <c r="I18" s="119" t="s">
         <v>208</v>
       </c>
-      <c r="J18" s="153"/>
-      <c r="K18" s="153"/>
-      <c r="L18" s="154"/>
-      <c r="M18" s="154"/>
-      <c r="N18" s="153"/>
-      <c r="O18" s="153"/>
-      <c r="P18" s="154"/>
-      <c r="Q18" s="154"/>
+      <c r="J18" s="150"/>
+      <c r="K18" s="150"/>
+      <c r="L18" s="151"/>
+      <c r="M18" s="151"/>
+      <c r="N18" s="150"/>
+      <c r="O18" s="150"/>
+      <c r="P18" s="151"/>
+      <c r="Q18" s="151"/>
       <c r="R18" s="43"/>
     </row>
     <row r="19" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="89" t="s">
         <v>149</v>
       </c>
-      <c r="B19" s="177"/>
-      <c r="C19" s="178"/>
-      <c r="D19" s="178"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
       <c r="E19" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="179"/>
-      <c r="G19" s="182"/>
-      <c r="H19" s="179"/>
+      <c r="F19" s="176"/>
+      <c r="G19" s="179"/>
+      <c r="H19" s="176"/>
       <c r="I19" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="J19" s="153"/>
-      <c r="K19" s="153"/>
-      <c r="L19" s="154"/>
-      <c r="M19" s="154"/>
-      <c r="N19" s="153"/>
-      <c r="O19" s="153"/>
-      <c r="P19" s="154"/>
-      <c r="Q19" s="154"/>
+      <c r="J19" s="150"/>
+      <c r="K19" s="150"/>
+      <c r="L19" s="151"/>
+      <c r="M19" s="151"/>
+      <c r="N19" s="150"/>
+      <c r="O19" s="150"/>
+      <c r="P19" s="151"/>
+      <c r="Q19" s="151"/>
       <c r="R19" s="43"/>
     </row>
     <row r="20" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="88" t="s">
         <v>141</v>
       </c>
-      <c r="B20" s="177"/>
-      <c r="C20" s="178" t="s">
+      <c r="B20" s="174"/>
+      <c r="C20" s="175" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="178"/>
+      <c r="D20" s="175"/>
       <c r="E20" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="179"/>
-      <c r="G20" s="183" t="s">
+      <c r="F20" s="176"/>
+      <c r="G20" s="180" t="s">
         <v>421</v>
       </c>
-      <c r="H20" s="184"/>
+      <c r="H20" s="181"/>
       <c r="I20" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="J20" s="153"/>
-      <c r="K20" s="153"/>
-      <c r="L20" s="154"/>
-      <c r="M20" s="154"/>
-      <c r="N20" s="153"/>
-      <c r="O20" s="153"/>
-      <c r="P20" s="154"/>
-      <c r="Q20" s="154"/>
+      <c r="J20" s="150"/>
+      <c r="K20" s="150"/>
+      <c r="L20" s="151"/>
+      <c r="M20" s="151"/>
+      <c r="N20" s="150"/>
+      <c r="O20" s="150"/>
+      <c r="P20" s="151"/>
+      <c r="Q20" s="151"/>
       <c r="R20" s="43"/>
     </row>
     <row r="21" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="88" t="s">
         <v>424</v>
       </c>
-      <c r="B21" s="177"/>
-      <c r="C21" s="178"/>
-      <c r="D21" s="178"/>
+      <c r="B21" s="174"/>
+      <c r="C21" s="175"/>
+      <c r="D21" s="175"/>
       <c r="E21" s="74" t="s">
         <v>425</v>
       </c>
-      <c r="F21" s="179"/>
-      <c r="G21" s="185"/>
-      <c r="H21" s="186"/>
+      <c r="F21" s="176"/>
+      <c r="G21" s="182"/>
+      <c r="H21" s="183"/>
       <c r="I21" s="69" t="s">
         <v>426</v>
       </c>
-      <c r="J21" s="153"/>
-      <c r="K21" s="153"/>
-      <c r="L21" s="154"/>
-      <c r="M21" s="154"/>
-      <c r="N21" s="153"/>
-      <c r="O21" s="153"/>
-      <c r="P21" s="154"/>
-      <c r="Q21" s="154"/>
+      <c r="J21" s="150"/>
+      <c r="K21" s="150"/>
+      <c r="L21" s="151"/>
+      <c r="M21" s="151"/>
+      <c r="N21" s="150"/>
+      <c r="O21" s="150"/>
+      <c r="P21" s="151"/>
+      <c r="Q21" s="151"/>
       <c r="R21" s="43"/>
     </row>
     <row r="22" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="89" t="s">
         <v>142</v>
       </c>
-      <c r="B22" s="177"/>
-      <c r="C22" s="178" t="s">
+      <c r="B22" s="174"/>
+      <c r="C22" s="175" t="s">
         <v>59</v>
       </c>
-      <c r="D22" s="178"/>
+      <c r="D22" s="175"/>
       <c r="E22" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="F22" s="179"/>
-      <c r="G22" s="183" t="s">
+      <c r="F22" s="176"/>
+      <c r="G22" s="180" t="s">
         <v>422</v>
       </c>
-      <c r="H22" s="184"/>
+      <c r="H22" s="181"/>
       <c r="I22" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="J22" s="153"/>
-      <c r="K22" s="153"/>
-      <c r="L22" s="154"/>
-      <c r="M22" s="154"/>
-      <c r="N22" s="153"/>
-      <c r="O22" s="153"/>
-      <c r="P22" s="154"/>
-      <c r="Q22" s="154"/>
+      <c r="J22" s="150"/>
+      <c r="K22" s="150"/>
+      <c r="L22" s="151"/>
+      <c r="M22" s="151"/>
+      <c r="N22" s="150"/>
+      <c r="O22" s="150"/>
+      <c r="P22" s="151"/>
+      <c r="Q22" s="151"/>
       <c r="R22" s="43"/>
     </row>
     <row r="23" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="89" t="s">
         <v>143</v>
       </c>
-      <c r="B23" s="177"/>
-      <c r="C23" s="178"/>
-      <c r="D23" s="178"/>
+      <c r="B23" s="174"/>
+      <c r="C23" s="175"/>
+      <c r="D23" s="175"/>
       <c r="E23" s="74" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="179"/>
-      <c r="G23" s="187"/>
-      <c r="H23" s="188"/>
+      <c r="F23" s="176"/>
+      <c r="G23" s="184"/>
+      <c r="H23" s="185"/>
       <c r="I23" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="J23" s="153"/>
-      <c r="K23" s="153"/>
-      <c r="L23" s="154"/>
-      <c r="M23" s="154"/>
-      <c r="N23" s="153"/>
-      <c r="O23" s="153"/>
-      <c r="P23" s="154"/>
-      <c r="Q23" s="154"/>
+      <c r="J23" s="150"/>
+      <c r="K23" s="150"/>
+      <c r="L23" s="151"/>
+      <c r="M23" s="151"/>
+      <c r="N23" s="150"/>
+      <c r="O23" s="150"/>
+      <c r="P23" s="151"/>
+      <c r="Q23" s="151"/>
       <c r="R23" s="43"/>
     </row>
     <row r="24" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="89" t="s">
         <v>173</v>
       </c>
-      <c r="B24" s="177"/>
-      <c r="C24" s="178"/>
-      <c r="D24" s="178"/>
+      <c r="B24" s="174"/>
+      <c r="C24" s="175"/>
+      <c r="D24" s="175"/>
       <c r="E24" s="74" t="s">
         <v>418</v>
       </c>
-      <c r="F24" s="179"/>
-      <c r="G24" s="185"/>
-      <c r="H24" s="186"/>
+      <c r="F24" s="176"/>
+      <c r="G24" s="182"/>
+      <c r="H24" s="183"/>
       <c r="I24" s="69" t="s">
         <v>356</v>
       </c>
-      <c r="J24" s="153"/>
-      <c r="K24" s="153"/>
-      <c r="L24" s="154"/>
-      <c r="M24" s="154"/>
-      <c r="N24" s="153"/>
-      <c r="O24" s="153"/>
-      <c r="P24" s="154"/>
-      <c r="Q24" s="154"/>
+      <c r="J24" s="150"/>
+      <c r="K24" s="150"/>
+      <c r="L24" s="151"/>
+      <c r="M24" s="151"/>
+      <c r="N24" s="150"/>
+      <c r="O24" s="150"/>
+      <c r="P24" s="151"/>
+      <c r="Q24" s="151"/>
       <c r="R24" s="43"/>
     </row>
     <row r="25" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="88" t="s">
         <v>150</v>
       </c>
-      <c r="B25" s="177"/>
-      <c r="C25" s="178" t="s">
+      <c r="B25" s="174"/>
+      <c r="C25" s="175" t="s">
         <v>60</v>
       </c>
-      <c r="D25" s="178"/>
+      <c r="D25" s="175"/>
       <c r="E25" s="74" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="179"/>
-      <c r="G25" s="183" t="s">
+      <c r="F25" s="176"/>
+      <c r="G25" s="180" t="s">
         <v>423</v>
       </c>
-      <c r="H25" s="184"/>
+      <c r="H25" s="181"/>
       <c r="I25" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="J25" s="153"/>
-      <c r="K25" s="153"/>
-      <c r="L25" s="154"/>
-      <c r="M25" s="154"/>
-      <c r="N25" s="153"/>
-      <c r="O25" s="153"/>
-      <c r="P25" s="154"/>
-      <c r="Q25" s="154"/>
+      <c r="J25" s="150"/>
+      <c r="K25" s="150"/>
+      <c r="L25" s="151"/>
+      <c r="M25" s="151"/>
+      <c r="N25" s="150"/>
+      <c r="O25" s="150"/>
+      <c r="P25" s="151"/>
+      <c r="Q25" s="151"/>
       <c r="R25" s="43"/>
     </row>
     <row r="26" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="88" t="s">
         <v>151</v>
       </c>
-      <c r="B26" s="177"/>
-      <c r="C26" s="178"/>
-      <c r="D26" s="178"/>
+      <c r="B26" s="174"/>
+      <c r="C26" s="175"/>
+      <c r="D26" s="175"/>
       <c r="E26" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="F26" s="179"/>
-      <c r="G26" s="187"/>
-      <c r="H26" s="188"/>
+      <c r="F26" s="176"/>
+      <c r="G26" s="184"/>
+      <c r="H26" s="185"/>
       <c r="I26" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="J26" s="153"/>
-      <c r="K26" s="153"/>
-      <c r="L26" s="154"/>
-      <c r="M26" s="154"/>
-      <c r="N26" s="153"/>
-      <c r="O26" s="153"/>
-      <c r="P26" s="154"/>
-      <c r="Q26" s="154"/>
+      <c r="J26" s="150"/>
+      <c r="K26" s="150"/>
+      <c r="L26" s="151"/>
+      <c r="M26" s="151"/>
+      <c r="N26" s="150"/>
+      <c r="O26" s="150"/>
+      <c r="P26" s="151"/>
+      <c r="Q26" s="151"/>
       <c r="R26" s="43"/>
     </row>
     <row r="27" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="B27" s="177"/>
-      <c r="C27" s="178"/>
-      <c r="D27" s="178"/>
+      <c r="B27" s="174"/>
+      <c r="C27" s="175"/>
+      <c r="D27" s="175"/>
       <c r="E27" s="74" t="s">
         <v>418</v>
       </c>
-      <c r="F27" s="179"/>
-      <c r="G27" s="185"/>
-      <c r="H27" s="186"/>
+      <c r="F27" s="176"/>
+      <c r="G27" s="182"/>
+      <c r="H27" s="183"/>
       <c r="I27" s="69" t="s">
         <v>356</v>
       </c>
-      <c r="J27" s="153"/>
-      <c r="K27" s="153"/>
-      <c r="L27" s="154"/>
-      <c r="M27" s="154"/>
-      <c r="N27" s="153"/>
-      <c r="O27" s="153"/>
-      <c r="P27" s="154"/>
-      <c r="Q27" s="154"/>
+      <c r="J27" s="150"/>
+      <c r="K27" s="150"/>
+      <c r="L27" s="151"/>
+      <c r="M27" s="151"/>
+      <c r="N27" s="150"/>
+      <c r="O27" s="150"/>
+      <c r="P27" s="151"/>
+      <c r="Q27" s="151"/>
       <c r="R27" s="43"/>
     </row>
     <row r="28" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="89" t="s">
         <v>152</v>
       </c>
-      <c r="B28" s="177" t="s">
+      <c r="B28" s="174" t="s">
         <v>417</v>
       </c>
-      <c r="C28" s="178" t="s">
+      <c r="C28" s="175" t="s">
         <v>57</v>
       </c>
-      <c r="D28" s="178" t="s">
+      <c r="D28" s="175" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="F28" s="179" t="s">
+      <c r="F28" s="176" t="s">
         <v>358</v>
       </c>
-      <c r="G28" s="180" t="s">
+      <c r="G28" s="177" t="s">
         <v>205</v>
       </c>
-      <c r="H28" s="179" t="s">
+      <c r="H28" s="176" t="s">
         <v>207</v>
       </c>
       <c r="I28" s="84" t="s">
         <v>178</v>
       </c>
-      <c r="J28" s="153"/>
-      <c r="K28" s="153"/>
-      <c r="L28" s="154"/>
-      <c r="M28" s="154"/>
-      <c r="N28" s="153"/>
-      <c r="O28" s="153"/>
-      <c r="P28" s="154"/>
-      <c r="Q28" s="154"/>
+      <c r="J28" s="150"/>
+      <c r="K28" s="150"/>
+      <c r="L28" s="151"/>
+      <c r="M28" s="151"/>
+      <c r="N28" s="150"/>
+      <c r="O28" s="150"/>
+      <c r="P28" s="151"/>
+      <c r="Q28" s="151"/>
       <c r="R28" s="43"/>
     </row>
     <row r="29" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="89" t="s">
         <v>153</v>
       </c>
-      <c r="B29" s="177"/>
-      <c r="C29" s="178"/>
-      <c r="D29" s="178"/>
+      <c r="B29" s="174"/>
+      <c r="C29" s="175"/>
+      <c r="D29" s="175"/>
       <c r="E29" s="117" t="s">
         <v>50</v>
       </c>
-      <c r="F29" s="179"/>
-      <c r="G29" s="181"/>
-      <c r="H29" s="179"/>
+      <c r="F29" s="176"/>
+      <c r="G29" s="178"/>
+      <c r="H29" s="176"/>
       <c r="I29" s="119" t="s">
         <v>50</v>
       </c>
-      <c r="J29" s="153"/>
-      <c r="K29" s="153"/>
-      <c r="L29" s="154"/>
-      <c r="M29" s="154"/>
-      <c r="N29" s="153"/>
-      <c r="O29" s="153"/>
-      <c r="P29" s="154"/>
-      <c r="Q29" s="154"/>
+      <c r="J29" s="150"/>
+      <c r="K29" s="150"/>
+      <c r="L29" s="151"/>
+      <c r="M29" s="151"/>
+      <c r="N29" s="150"/>
+      <c r="O29" s="150"/>
+      <c r="P29" s="151"/>
+      <c r="Q29" s="151"/>
       <c r="R29" s="43"/>
     </row>
     <row r="30" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="89" t="s">
         <v>154</v>
       </c>
-      <c r="B30" s="177"/>
-      <c r="C30" s="178"/>
-      <c r="D30" s="178" t="s">
+      <c r="B30" s="174"/>
+      <c r="C30" s="175"/>
+      <c r="D30" s="175" t="s">
         <v>15</v>
       </c>
       <c r="E30" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="179"/>
-      <c r="G30" s="181"/>
-      <c r="H30" s="179" t="s">
+      <c r="F30" s="176"/>
+      <c r="G30" s="178"/>
+      <c r="H30" s="176" t="s">
         <v>206</v>
       </c>
       <c r="I30" s="69" t="s">
         <v>178</v>
       </c>
-      <c r="J30" s="153"/>
-      <c r="K30" s="153"/>
-      <c r="L30" s="154"/>
-      <c r="M30" s="154"/>
-      <c r="N30" s="153"/>
-      <c r="O30" s="153"/>
-      <c r="P30" s="154"/>
-      <c r="Q30" s="154"/>
+      <c r="J30" s="150"/>
+      <c r="K30" s="150"/>
+      <c r="L30" s="151"/>
+      <c r="M30" s="151"/>
+      <c r="N30" s="150"/>
+      <c r="O30" s="150"/>
+      <c r="P30" s="151"/>
+      <c r="Q30" s="151"/>
       <c r="R30" s="43"/>
     </row>
     <row r="31" spans="1:18" s="3" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="89" t="s">
         <v>155</v>
       </c>
-      <c r="B31" s="177"/>
-      <c r="C31" s="178"/>
-      <c r="D31" s="178"/>
+      <c r="B31" s="174"/>
+      <c r="C31" s="175"/>
+      <c r="D31" s="175"/>
       <c r="E31" s="75" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="179"/>
-      <c r="G31" s="182"/>
-      <c r="H31" s="179"/>
+      <c r="F31" s="176"/>
+      <c r="G31" s="179"/>
+      <c r="H31" s="176"/>
       <c r="I31" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="J31" s="153"/>
-      <c r="K31" s="153"/>
-      <c r="L31" s="154"/>
-      <c r="M31" s="154"/>
-      <c r="N31" s="153"/>
-      <c r="O31" s="153"/>
-      <c r="P31" s="154"/>
-      <c r="Q31" s="154"/>
+      <c r="J31" s="150"/>
+      <c r="K31" s="150"/>
+      <c r="L31" s="151"/>
+      <c r="M31" s="151"/>
+      <c r="N31" s="150"/>
+      <c r="O31" s="150"/>
+      <c r="P31" s="151"/>
+      <c r="Q31" s="151"/>
       <c r="R31" s="43"/>
     </row>
     <row r="32" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.2">
@@ -8758,7 +8752,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="156"/>
+    <col min="1" max="1" width="9.140625" style="153"/>
     <col min="2" max="2" width="14.140625" style="56" customWidth="1"/>
     <col min="3" max="3" width="25.5703125" style="56" customWidth="1"/>
     <col min="4" max="9" width="21.140625" style="56" customWidth="1"/>
@@ -8798,28 +8792,28 @@
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B5" s="86"/>
       <c r="C5" s="86"/>
-      <c r="D5" s="192" t="s">
+      <c r="D5" s="189" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="192"/>
-      <c r="F5" s="192"/>
-      <c r="G5" s="192"/>
-      <c r="H5" s="192"/>
-      <c r="I5" s="192"/>
+      <c r="E5" s="189"/>
+      <c r="F5" s="189"/>
+      <c r="G5" s="189"/>
+      <c r="H5" s="189"/>
+      <c r="I5" s="189"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B6" s="86"/>
       <c r="C6" s="86"/>
-      <c r="D6" s="193" t="s">
+      <c r="D6" s="190" t="s">
         <v>61</v>
       </c>
-      <c r="E6" s="193"/>
-      <c r="F6" s="193"/>
-      <c r="G6" s="194" t="s">
+      <c r="E6" s="190"/>
+      <c r="F6" s="190"/>
+      <c r="G6" s="191" t="s">
         <v>63</v>
       </c>
-      <c r="H6" s="194"/>
-      <c r="I6" s="194"/>
+      <c r="H6" s="191"/>
+      <c r="I6" s="191"/>
     </row>
     <row r="7" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B7" s="86"/>
@@ -8846,53 +8840,53 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B8" s="86"/>
       <c r="C8" s="86"/>
-      <c r="D8" s="195" t="s">
+      <c r="D8" s="192" t="s">
         <v>205</v>
       </c>
-      <c r="E8" s="195"/>
-      <c r="F8" s="195"/>
-      <c r="G8" s="195"/>
-      <c r="H8" s="195"/>
-      <c r="I8" s="195"/>
+      <c r="E8" s="192"/>
+      <c r="F8" s="192"/>
+      <c r="G8" s="192"/>
+      <c r="H8" s="192"/>
+      <c r="I8" s="192"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B9" s="86"/>
       <c r="C9" s="86"/>
-      <c r="D9" s="195" t="s">
+      <c r="D9" s="192" t="s">
         <v>432</v>
       </c>
-      <c r="E9" s="195"/>
-      <c r="F9" s="195"/>
-      <c r="G9" s="195" t="s">
+      <c r="E9" s="192"/>
+      <c r="F9" s="192"/>
+      <c r="G9" s="192" t="s">
         <v>209</v>
       </c>
-      <c r="H9" s="195"/>
-      <c r="I9" s="195"/>
+      <c r="H9" s="192"/>
+      <c r="I9" s="192"/>
     </row>
     <row r="10" spans="1:10" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B10" s="121"/>
       <c r="C10" s="121"/>
-      <c r="D10" s="155" t="s">
+      <c r="D10" s="152" t="s">
         <v>210</v>
       </c>
-      <c r="E10" s="155" t="s">
+      <c r="E10" s="152" t="s">
         <v>50</v>
       </c>
-      <c r="F10" s="155" t="s">
+      <c r="F10" s="152" t="s">
         <v>208</v>
       </c>
-      <c r="G10" s="155" t="s">
+      <c r="G10" s="152" t="s">
         <v>210</v>
       </c>
-      <c r="H10" s="155" t="s">
+      <c r="H10" s="152" t="s">
         <v>50</v>
       </c>
-      <c r="I10" s="155" t="s">
+      <c r="I10" s="152" t="s">
         <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="156" t="s">
+      <c r="A11" s="153" t="s">
         <v>462</v>
       </c>
       <c r="B11" s="93" t="s">
@@ -8910,7 +8904,7 @@
       <c r="J11" s="11"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="156" t="s">
+      <c r="A12" s="153" t="s">
         <v>463</v>
       </c>
       <c r="B12" s="93" t="s">
@@ -8928,7 +8922,7 @@
       <c r="J12" s="11"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="156" t="s">
+      <c r="A13" s="153" t="s">
         <v>464</v>
       </c>
       <c r="B13" s="93" t="s">
@@ -8946,7 +8940,7 @@
       <c r="J13" s="11"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A14" s="156" t="s">
+      <c r="A14" s="153" t="s">
         <v>465</v>
       </c>
       <c r="B14" s="93" t="s">
@@ -8964,7 +8958,7 @@
       <c r="J14" s="11"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="156" t="s">
+      <c r="A15" s="153" t="s">
         <v>466</v>
       </c>
       <c r="B15" s="93" t="s">
@@ -8982,7 +8976,7 @@
       <c r="J15" s="11"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="156" t="s">
+      <c r="A16" s="153" t="s">
         <v>467</v>
       </c>
       <c r="B16" s="93" t="s">
@@ -9000,7 +8994,7 @@
       <c r="J16" s="11"/>
     </row>
     <row r="17" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="156" t="s">
+      <c r="A17" s="153" t="s">
         <v>468</v>
       </c>
       <c r="B17" s="93" t="s">
@@ -9018,7 +9012,7 @@
       <c r="J17" s="11"/>
     </row>
     <row r="18" spans="1:10" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="156" t="s">
+      <c r="A18" s="153" t="s">
         <v>469</v>
       </c>
       <c r="B18" s="93" t="s">
@@ -9036,7 +9030,7 @@
       <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="156" t="s">
+      <c r="A19" s="153" t="s">
         <v>470</v>
       </c>
       <c r="B19" s="93" t="s">
@@ -9054,7 +9048,7 @@
       <c r="J19" s="11"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="156" t="s">
+      <c r="A20" s="153" t="s">
         <v>471</v>
       </c>
       <c r="B20" s="93" t="s">
@@ -9072,7 +9066,7 @@
       <c r="J20" s="11"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="153" t="s">
         <v>472</v>
       </c>
       <c r="B21" s="93" t="s">
@@ -9090,7 +9084,7 @@
       <c r="J21" s="11"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="156" t="s">
+      <c r="A22" s="153" t="s">
         <v>473</v>
       </c>
       <c r="B22" s="93" t="s">
@@ -9108,7 +9102,7 @@
       <c r="J22" s="11"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="156" t="s">
+      <c r="A23" s="153" t="s">
         <v>474</v>
       </c>
       <c r="B23" s="93" t="s">
@@ -9126,7 +9120,7 @@
       <c r="J23" s="11"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="156" t="s">
+      <c r="A24" s="153" t="s">
         <v>475</v>
       </c>
       <c r="B24" s="93" t="s">
@@ -9144,7 +9138,7 @@
       <c r="J24" s="11"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="153" t="s">
         <v>476</v>
       </c>
       <c r="B25" s="93" t="s">
@@ -9162,7 +9156,7 @@
       <c r="J25" s="11"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="156" t="s">
+      <c r="A26" s="153" t="s">
         <v>477</v>
       </c>
       <c r="B26" s="93" t="s">
@@ -9180,7 +9174,7 @@
       <c r="J26" s="11"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="156" t="s">
+      <c r="A27" s="153" t="s">
         <v>478</v>
       </c>
       <c r="B27" s="93" t="s">
@@ -9198,7 +9192,7 @@
       <c r="J27" s="11"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="156" t="s">
+      <c r="A28" s="153" t="s">
         <v>479</v>
       </c>
       <c r="B28" s="93" t="s">
@@ -9216,7 +9210,7 @@
       <c r="J28" s="11"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="156" t="s">
+      <c r="A29" s="153" t="s">
         <v>480</v>
       </c>
       <c r="B29" s="93" t="s">
@@ -9234,7 +9228,7 @@
       <c r="J29" s="11"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="156" t="s">
+      <c r="A30" s="153" t="s">
         <v>481</v>
       </c>
       <c r="B30" s="93" t="s">
@@ -9252,7 +9246,7 @@
       <c r="J30" s="11"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="156" t="s">
+      <c r="A31" s="153" t="s">
         <v>482</v>
       </c>
       <c r="B31" s="93" t="s">
@@ -9270,7 +9264,7 @@
       <c r="J31" s="11"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="156" t="s">
+      <c r="A32" s="153" t="s">
         <v>483</v>
       </c>
       <c r="B32" s="93" t="s">
@@ -9288,7 +9282,7 @@
       <c r="J32" s="11"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="156" t="s">
+      <c r="A33" s="153" t="s">
         <v>484</v>
       </c>
       <c r="B33" s="93" t="s">
@@ -9306,7 +9300,7 @@
       <c r="J33" s="11"/>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="156" t="s">
+      <c r="A34" s="153" t="s">
         <v>485</v>
       </c>
       <c r="B34" s="93" t="s">
@@ -9324,7 +9318,7 @@
       <c r="J34" s="11"/>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="156" t="s">
+      <c r="A35" s="153" t="s">
         <v>486</v>
       </c>
       <c r="B35" s="93" t="s">
@@ -9342,7 +9336,7 @@
       <c r="J35" s="11"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="156" t="s">
+      <c r="A36" s="153" t="s">
         <v>487</v>
       </c>
       <c r="B36" s="93" t="s">
@@ -9360,7 +9354,7 @@
       <c r="J36" s="11"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A37" s="156" t="s">
+      <c r="A37" s="153" t="s">
         <v>488</v>
       </c>
       <c r="B37" s="93" t="s">
@@ -9378,7 +9372,7 @@
       <c r="J37" s="11"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A38" s="156" t="s">
+      <c r="A38" s="153" t="s">
         <v>489</v>
       </c>
       <c r="B38" s="93" t="s">
@@ -9396,7 +9390,7 @@
       <c r="J38" s="11"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="156" t="s">
+      <c r="A39" s="153" t="s">
         <v>490</v>
       </c>
       <c r="B39" s="93" t="s">
@@ -9429,7 +9423,7 @@
       <c r="J40" s="11"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41" s="156" t="s">
+      <c r="A41" s="153" t="s">
         <v>491</v>
       </c>
       <c r="B41" s="93" t="s">
@@ -9447,7 +9441,7 @@
       <c r="J41" s="11"/>
     </row>
     <row r="42" spans="1:10" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="156" t="s">
+      <c r="A42" s="153" t="s">
         <v>493</v>
       </c>
       <c r="B42" s="93" t="s">
@@ -9465,7 +9459,7 @@
       <c r="J42" s="11"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43" s="156" t="s">
+      <c r="A43" s="153" t="s">
         <v>494</v>
       </c>
       <c r="B43" s="93" t="s">
@@ -9483,7 +9477,7 @@
       <c r="J43" s="11"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44" s="156" t="s">
+      <c r="A44" s="153" t="s">
         <v>496</v>
       </c>
       <c r="B44" s="93" t="s">
@@ -9501,7 +9495,7 @@
       <c r="J44" s="11"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45" s="156" t="s">
+      <c r="A45" s="153" t="s">
         <v>498</v>
       </c>
       <c r="B45" s="93" t="s">
@@ -9519,7 +9513,7 @@
       <c r="J45" s="11"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46" s="156" t="s">
+      <c r="A46" s="153" t="s">
         <v>500</v>
       </c>
       <c r="B46" s="93" t="s">
@@ -9537,7 +9531,7 @@
       <c r="J46" s="11"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47" s="156" t="s">
+      <c r="A47" s="153" t="s">
         <v>502</v>
       </c>
       <c r="B47" s="93" t="s">
@@ -9555,7 +9549,7 @@
       <c r="J47" s="11"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48" s="156" t="s">
+      <c r="A48" s="153" t="s">
         <v>503</v>
       </c>
       <c r="B48" s="93" t="s">
@@ -9573,7 +9567,7 @@
       <c r="J48" s="11"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" s="156" t="s">
+      <c r="A49" s="153" t="s">
         <v>504</v>
       </c>
       <c r="B49" s="93" t="s">
@@ -9591,7 +9585,7 @@
       <c r="J49" s="11"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50" s="156" t="s">
+      <c r="A50" s="153" t="s">
         <v>505</v>
       </c>
       <c r="B50" s="93" t="s">
@@ -9609,7 +9603,7 @@
       <c r="J50" s="11"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="156" t="s">
+      <c r="A51" s="153" t="s">
         <v>507</v>
       </c>
       <c r="B51" s="93" t="s">
@@ -9627,7 +9621,7 @@
       <c r="J51" s="11"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="156" t="s">
+      <c r="A52" s="153" t="s">
         <v>510</v>
       </c>
       <c r="B52" s="93" t="s">
@@ -9645,7 +9639,7 @@
       <c r="J52" s="11"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53" s="156" t="s">
+      <c r="A53" s="153" t="s">
         <v>512</v>
       </c>
       <c r="B53" s="93" t="s">
@@ -9663,7 +9657,7 @@
       <c r="J53" s="11"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="156" t="s">
+      <c r="A54" s="153" t="s">
         <v>514</v>
       </c>
       <c r="B54" s="93" t="s">
@@ -9681,7 +9675,7 @@
       <c r="J54" s="11"/>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55" s="156" t="s">
+      <c r="A55" s="153" t="s">
         <v>516</v>
       </c>
       <c r="B55" s="93" t="s">
@@ -9699,7 +9693,7 @@
       <c r="J55" s="11"/>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56" s="156" t="s">
+      <c r="A56" s="153" t="s">
         <v>517</v>
       </c>
       <c r="B56" s="93" t="s">
@@ -9717,7 +9711,7 @@
       <c r="J56" s="11"/>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57" s="156" t="s">
+      <c r="A57" s="153" t="s">
         <v>519</v>
       </c>
       <c r="B57" s="93" t="s">
@@ -9735,7 +9729,7 @@
       <c r="J57" s="11"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58" s="156" t="s">
+      <c r="A58" s="153" t="s">
         <v>521</v>
       </c>
       <c r="B58" s="93" t="s">
@@ -9753,7 +9747,7 @@
       <c r="J58" s="11"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59" s="156" t="s">
+      <c r="A59" s="153" t="s">
         <v>523</v>
       </c>
       <c r="B59" s="93" t="s">
@@ -9771,7 +9765,7 @@
       <c r="J59" s="11"/>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60" s="156" t="s">
+      <c r="A60" s="153" t="s">
         <v>524</v>
       </c>
       <c r="B60" s="93" t="s">
@@ -9789,7 +9783,7 @@
       <c r="J60" s="11"/>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="156" t="s">
+      <c r="A61" s="153" t="s">
         <v>526</v>
       </c>
       <c r="B61" s="93" t="s">
@@ -9807,7 +9801,7 @@
       <c r="J61" s="11"/>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62" s="156" t="s">
+      <c r="A62" s="153" t="s">
         <v>527</v>
       </c>
       <c r="B62" s="93" t="s">
@@ -9825,7 +9819,7 @@
       <c r="J62" s="11"/>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" s="156" t="s">
+      <c r="A63" s="153" t="s">
         <v>529</v>
       </c>
       <c r="B63" s="93" t="s">
@@ -9843,7 +9837,7 @@
       <c r="J63" s="11"/>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" s="156" t="s">
+      <c r="A64" s="153" t="s">
         <v>531</v>
       </c>
       <c r="B64" s="93" t="s">
@@ -9861,7 +9855,7 @@
       <c r="J64" s="11"/>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A65" s="156" t="s">
+      <c r="A65" s="153" t="s">
         <v>533</v>
       </c>
       <c r="B65" s="93" t="s">
@@ -9879,7 +9873,7 @@
       <c r="J65" s="11"/>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A66" s="156" t="s">
+      <c r="A66" s="153" t="s">
         <v>535</v>
       </c>
       <c r="B66" s="93" t="s">
@@ -9897,7 +9891,7 @@
       <c r="J66" s="11"/>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A67" s="156" t="s">
+      <c r="A67" s="153" t="s">
         <v>538</v>
       </c>
       <c r="B67" s="93" t="s">
@@ -9915,7 +9909,7 @@
       <c r="J67" s="11"/>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A68" s="156" t="s">
+      <c r="A68" s="153" t="s">
         <v>539</v>
       </c>
       <c r="B68" s="93" t="s">
@@ -9933,7 +9927,7 @@
       <c r="J68" s="11"/>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A69" s="156" t="s">
+      <c r="A69" s="153" t="s">
         <v>541</v>
       </c>
       <c r="B69" s="93" t="s">
@@ -9951,7 +9945,7 @@
       <c r="J69" s="11"/>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A70" s="156" t="s">
+      <c r="A70" s="153" t="s">
         <v>543</v>
       </c>
       <c r="B70" s="93" t="s">
@@ -9969,7 +9963,7 @@
       <c r="J70" s="11"/>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A71" s="156" t="s">
+      <c r="A71" s="153" t="s">
         <v>546</v>
       </c>
       <c r="B71" s="93" t="s">
@@ -9987,7 +9981,7 @@
       <c r="J71" s="11"/>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A72" s="156" t="s">
+      <c r="A72" s="153" t="s">
         <v>549</v>
       </c>
       <c r="B72" s="93" t="s">
@@ -10005,7 +9999,7 @@
       <c r="J72" s="11"/>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A73" s="156" t="s">
+      <c r="A73" s="153" t="s">
         <v>551</v>
       </c>
       <c r="B73" s="93" t="s">
@@ -10023,7 +10017,7 @@
       <c r="J73" s="11"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A74" s="156" t="s">
+      <c r="A74" s="153" t="s">
         <v>554</v>
       </c>
       <c r="B74" s="93" t="s">
@@ -10041,7 +10035,7 @@
       <c r="J74" s="11"/>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A75" s="156" t="s">
+      <c r="A75" s="153" t="s">
         <v>557</v>
       </c>
       <c r="B75" s="93" t="s">
@@ -10059,7 +10053,7 @@
       <c r="J75" s="11"/>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A76" s="156" t="s">
+      <c r="A76" s="153" t="s">
         <v>559</v>
       </c>
       <c r="B76" s="93" t="s">
@@ -10077,7 +10071,7 @@
       <c r="J76" s="11"/>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A77" s="156" t="s">
+      <c r="A77" s="153" t="s">
         <v>561</v>
       </c>
       <c r="B77" s="93" t="s">
@@ -10095,7 +10089,7 @@
       <c r="J77" s="11"/>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A78" s="156" t="s">
+      <c r="A78" s="153" t="s">
         <v>563</v>
       </c>
       <c r="B78" s="93" t="s">
@@ -10113,7 +10107,7 @@
       <c r="J78" s="11"/>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A79" s="156" t="s">
+      <c r="A79" s="153" t="s">
         <v>566</v>
       </c>
       <c r="B79" s="93" t="s">
@@ -10131,7 +10125,7 @@
       <c r="J79" s="11"/>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A80" s="156" t="s">
+      <c r="A80" s="153" t="s">
         <v>568</v>
       </c>
       <c r="B80" s="93" t="s">
@@ -10149,7 +10143,7 @@
       <c r="J80" s="11"/>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A81" s="156" t="s">
+      <c r="A81" s="153" t="s">
         <v>569</v>
       </c>
       <c r="B81" s="93" t="s">
@@ -10167,7 +10161,7 @@
       <c r="J81" s="11"/>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A82" s="156" t="s">
+      <c r="A82" s="153" t="s">
         <v>570</v>
       </c>
       <c r="B82" s="93" t="s">
@@ -10185,7 +10179,7 @@
       <c r="J82" s="11"/>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A83" s="156" t="s">
+      <c r="A83" s="153" t="s">
         <v>571</v>
       </c>
       <c r="B83" s="93" t="s">
@@ -10203,7 +10197,7 @@
       <c r="J83" s="11"/>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A84" s="156" t="s">
+      <c r="A84" s="153" t="s">
         <v>573</v>
       </c>
       <c r="B84" s="93" t="s">
@@ -10221,7 +10215,7 @@
       <c r="J84" s="11"/>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A85" s="156" t="s">
+      <c r="A85" s="153" t="s">
         <v>576</v>
       </c>
       <c r="B85" s="93" t="s">
@@ -10239,7 +10233,7 @@
       <c r="J85" s="11"/>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A86" s="156" t="s">
+      <c r="A86" s="153" t="s">
         <v>577</v>
       </c>
       <c r="B86" s="93" t="s">
@@ -10257,7 +10251,7 @@
       <c r="J86" s="11"/>
     </row>
     <row r="87" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A87" s="156" t="s">
+      <c r="A87" s="153" t="s">
         <v>579</v>
       </c>
       <c r="B87" s="93" t="s">
@@ -10275,7 +10269,7 @@
       <c r="J87" s="11"/>
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A88" s="156" t="s">
+      <c r="A88" s="153" t="s">
         <v>581</v>
       </c>
       <c r="B88" s="93" t="s">
@@ -10293,7 +10287,7 @@
       <c r="J88" s="11"/>
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A89" s="156" t="s">
+      <c r="A89" s="153" t="s">
         <v>583</v>
       </c>
       <c r="B89" s="93" t="s">
@@ -10311,7 +10305,7 @@
       <c r="J89" s="11"/>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A90" s="156" t="s">
+      <c r="A90" s="153" t="s">
         <v>585</v>
       </c>
       <c r="B90" s="93" t="s">
@@ -10329,7 +10323,7 @@
       <c r="J90" s="11"/>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A91" s="156" t="s">
+      <c r="A91" s="153" t="s">
         <v>587</v>
       </c>
       <c r="B91" s="93" t="s">
@@ -10347,7 +10341,7 @@
       <c r="J91" s="11"/>
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A92" s="156" t="s">
+      <c r="A92" s="153" t="s">
         <v>589</v>
       </c>
       <c r="B92" s="93" t="s">
@@ -10365,7 +10359,7 @@
       <c r="J92" s="11"/>
     </row>
     <row r="93" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A93" s="156" t="s">
+      <c r="A93" s="153" t="s">
         <v>591</v>
       </c>
       <c r="B93" s="93" t="s">
@@ -10383,7 +10377,7 @@
       <c r="J93" s="11"/>
     </row>
     <row r="94" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A94" s="156" t="s">
+      <c r="A94" s="153" t="s">
         <v>593</v>
       </c>
       <c r="B94" s="93" t="s">
@@ -10401,7 +10395,7 @@
       <c r="J94" s="11"/>
     </row>
     <row r="95" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A95" s="156" t="s">
+      <c r="A95" s="153" t="s">
         <v>595</v>
       </c>
       <c r="B95" s="93" t="s">
@@ -10419,7 +10413,7 @@
       <c r="J95" s="11"/>
     </row>
     <row r="96" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A96" s="156" t="s">
+      <c r="A96" s="153" t="s">
         <v>597</v>
       </c>
       <c r="B96" s="93" t="s">
@@ -10437,7 +10431,7 @@
       <c r="J96" s="11"/>
     </row>
     <row r="97" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A97" s="156" t="s">
+      <c r="A97" s="153" t="s">
         <v>600</v>
       </c>
       <c r="B97" s="93" t="s">
@@ -10455,7 +10449,7 @@
       <c r="J97" s="11"/>
     </row>
     <row r="98" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A98" s="156" t="s">
+      <c r="A98" s="153" t="s">
         <v>602</v>
       </c>
       <c r="B98" s="93" t="s">
@@ -10473,7 +10467,7 @@
       <c r="J98" s="11"/>
     </row>
     <row r="99" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A99" s="156" t="s">
+      <c r="A99" s="153" t="s">
         <v>604</v>
       </c>
       <c r="B99" s="93" t="s">
@@ -10491,7 +10485,7 @@
       <c r="J99" s="11"/>
     </row>
     <row r="100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A100" s="156" t="s">
+      <c r="A100" s="153" t="s">
         <v>607</v>
       </c>
       <c r="B100" s="93" t="s">
@@ -10509,7 +10503,7 @@
       <c r="J100" s="11"/>
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A101" s="156" t="s">
+      <c r="A101" s="153" t="s">
         <v>609</v>
       </c>
       <c r="B101" s="93" t="s">
@@ -10527,7 +10521,7 @@
       <c r="J101" s="11"/>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A102" s="156" t="s">
+      <c r="A102" s="153" t="s">
         <v>611</v>
       </c>
       <c r="B102" s="93" t="s">
@@ -10545,7 +10539,7 @@
       <c r="J102" s="11"/>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A103" s="156" t="s">
+      <c r="A103" s="153" t="s">
         <v>613</v>
       </c>
       <c r="B103" s="93" t="s">
@@ -10563,7 +10557,7 @@
       <c r="J103" s="11"/>
     </row>
     <row r="104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="153" t="s">
         <v>615</v>
       </c>
       <c r="B104" s="93" t="s">
@@ -10581,7 +10575,7 @@
       <c r="J104" s="11"/>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A105" s="156" t="s">
+      <c r="A105" s="153" t="s">
         <v>617</v>
       </c>
       <c r="B105" s="93" t="s">
@@ -10599,7 +10593,7 @@
       <c r="J105" s="11"/>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A106" s="156" t="s">
+      <c r="A106" s="153" t="s">
         <v>618</v>
       </c>
       <c r="B106" s="93" t="s">
@@ -10617,7 +10611,7 @@
       <c r="J106" s="11"/>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A107" s="156" t="s">
+      <c r="A107" s="153" t="s">
         <v>620</v>
       </c>
       <c r="B107" s="93" t="s">
@@ -10635,7 +10629,7 @@
       <c r="J107" s="11"/>
     </row>
     <row r="108" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A108" s="156" t="s">
+      <c r="A108" s="153" t="s">
         <v>621</v>
       </c>
       <c r="B108" s="93" t="s">
@@ -10653,7 +10647,7 @@
       <c r="J108" s="11"/>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A109" s="156" t="s">
+      <c r="A109" s="153" t="s">
         <v>623</v>
       </c>
       <c r="B109" s="93" t="s">
@@ -10671,7 +10665,7 @@
       <c r="J109" s="11"/>
     </row>
     <row r="110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A110" s="156" t="s">
+      <c r="A110" s="153" t="s">
         <v>626</v>
       </c>
       <c r="B110" s="93" t="s">
@@ -10689,7 +10683,7 @@
       <c r="J110" s="11"/>
     </row>
     <row r="111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A111" s="156" t="s">
+      <c r="A111" s="153" t="s">
         <v>627</v>
       </c>
       <c r="B111" s="93" t="s">
@@ -10707,7 +10701,7 @@
       <c r="J111" s="11"/>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A112" s="156" t="s">
+      <c r="A112" s="153" t="s">
         <v>629</v>
       </c>
       <c r="B112" s="93" t="s">
@@ -10725,7 +10719,7 @@
       <c r="J112" s="11"/>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A113" s="156" t="s">
+      <c r="A113" s="153" t="s">
         <v>631</v>
       </c>
       <c r="B113" s="93" t="s">
@@ -10743,7 +10737,7 @@
       <c r="J113" s="11"/>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A114" s="156" t="s">
+      <c r="A114" s="153" t="s">
         <v>633</v>
       </c>
       <c r="B114" s="93" t="s">
@@ -10761,7 +10755,7 @@
       <c r="J114" s="11"/>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A115" s="156" t="s">
+      <c r="A115" s="153" t="s">
         <v>635</v>
       </c>
       <c r="B115" s="93" t="s">
@@ -10779,7 +10773,7 @@
       <c r="J115" s="11"/>
     </row>
     <row r="116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A116" s="156" t="s">
+      <c r="A116" s="153" t="s">
         <v>636</v>
       </c>
       <c r="B116" s="93" t="s">
@@ -10797,7 +10791,7 @@
       <c r="J116" s="11"/>
     </row>
     <row r="117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A117" s="156" t="s">
+      <c r="A117" s="153" t="s">
         <v>637</v>
       </c>
       <c r="B117" s="93" t="s">
@@ -10815,7 +10809,7 @@
       <c r="J117" s="11"/>
     </row>
     <row r="118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A118" s="156" t="s">
+      <c r="A118" s="153" t="s">
         <v>639</v>
       </c>
       <c r="B118" s="93" t="s">
@@ -10833,7 +10827,7 @@
       <c r="J118" s="11"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A119" s="156" t="s">
+      <c r="A119" s="153" t="s">
         <v>641</v>
       </c>
       <c r="B119" s="93" t="s">
@@ -10851,7 +10845,7 @@
       <c r="J119" s="11"/>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A120" s="156" t="s">
+      <c r="A120" s="153" t="s">
         <v>642</v>
       </c>
       <c r="B120" s="93" t="s">
@@ -10869,7 +10863,7 @@
       <c r="J120" s="11"/>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A121" s="156" t="s">
+      <c r="A121" s="153" t="s">
         <v>645</v>
       </c>
       <c r="B121" s="93" t="s">
@@ -10887,7 +10881,7 @@
       <c r="J121" s="11"/>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A122" s="156" t="s">
+      <c r="A122" s="153" t="s">
         <v>647</v>
       </c>
       <c r="B122" s="93" t="s">
@@ -10905,7 +10899,7 @@
       <c r="J122" s="11"/>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A123" s="156" t="s">
+      <c r="A123" s="153" t="s">
         <v>648</v>
       </c>
       <c r="B123" s="93" t="s">
@@ -10923,7 +10917,7 @@
       <c r="J123" s="11"/>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A124" s="156" t="s">
+      <c r="A124" s="153" t="s">
         <v>650</v>
       </c>
       <c r="B124" s="93" t="s">
@@ -10941,7 +10935,7 @@
       <c r="J124" s="11"/>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A125" s="156" t="s">
+      <c r="A125" s="153" t="s">
         <v>651</v>
       </c>
       <c r="B125" s="93" t="s">
@@ -10959,7 +10953,7 @@
       <c r="J125" s="11"/>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A126" s="156" t="s">
+      <c r="A126" s="153" t="s">
         <v>653</v>
       </c>
       <c r="B126" s="93" t="s">
@@ -10977,7 +10971,7 @@
       <c r="J126" s="11"/>
     </row>
     <row r="127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A127" s="156" t="s">
+      <c r="A127" s="153" t="s">
         <v>655</v>
       </c>
       <c r="B127" s="93" t="s">
@@ -10995,7 +10989,7 @@
       <c r="J127" s="11"/>
     </row>
     <row r="128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A128" s="156" t="s">
+      <c r="A128" s="153" t="s">
         <v>656</v>
       </c>
       <c r="B128" s="93" t="s">
@@ -11013,7 +11007,7 @@
       <c r="J128" s="11"/>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A129" s="156" t="s">
+      <c r="A129" s="153" t="s">
         <v>659</v>
       </c>
       <c r="B129" s="93" t="s">
@@ -11031,7 +11025,7 @@
       <c r="J129" s="11"/>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A130" s="156" t="s">
+      <c r="A130" s="153" t="s">
         <v>661</v>
       </c>
       <c r="B130" s="93" t="s">
@@ -11049,7 +11043,7 @@
       <c r="J130" s="11"/>
     </row>
     <row r="131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A131" s="156" t="s">
+      <c r="A131" s="153" t="s">
         <v>662</v>
       </c>
       <c r="B131" s="93" t="s">
@@ -11067,7 +11061,7 @@
       <c r="J131" s="11"/>
     </row>
     <row r="132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A132" s="156" t="s">
+      <c r="A132" s="153" t="s">
         <v>663</v>
       </c>
       <c r="B132" s="93" t="s">
@@ -11085,7 +11079,7 @@
       <c r="J132" s="11"/>
     </row>
     <row r="133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A133" s="156" t="s">
+      <c r="A133" s="153" t="s">
         <v>664</v>
       </c>
       <c r="B133" s="93" t="s">
@@ -11103,7 +11097,7 @@
       <c r="J133" s="11"/>
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A134" s="156" t="s">
+      <c r="A134" s="153" t="s">
         <v>666</v>
       </c>
       <c r="B134" s="93" t="s">
@@ -11121,7 +11115,7 @@
       <c r="J134" s="11"/>
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A135" s="156" t="s">
+      <c r="A135" s="153" t="s">
         <v>667</v>
       </c>
       <c r="B135" s="93" t="s">
@@ -11139,7 +11133,7 @@
       <c r="J135" s="11"/>
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A136" s="156" t="s">
+      <c r="A136" s="153" t="s">
         <v>668</v>
       </c>
       <c r="B136" s="93" t="s">
@@ -11157,7 +11151,7 @@
       <c r="J136" s="11"/>
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A137" s="156" t="s">
+      <c r="A137" s="153" t="s">
         <v>670</v>
       </c>
       <c r="B137" s="93" t="s">
@@ -11175,7 +11169,7 @@
       <c r="J137" s="11"/>
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A138" s="156" t="s">
+      <c r="A138" s="153" t="s">
         <v>672</v>
       </c>
       <c r="B138" s="93" t="s">
@@ -11193,7 +11187,7 @@
       <c r="J138" s="11"/>
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A139" s="156" t="s">
+      <c r="A139" s="153" t="s">
         <v>674</v>
       </c>
       <c r="B139" s="93" t="s">
@@ -11211,7 +11205,7 @@
       <c r="J139" s="11"/>
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A140" s="156" t="s">
+      <c r="A140" s="153" t="s">
         <v>676</v>
       </c>
       <c r="B140" s="93" t="s">
@@ -11229,7 +11223,7 @@
       <c r="J140" s="11"/>
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A141" s="156" t="s">
+      <c r="A141" s="153" t="s">
         <v>677</v>
       </c>
       <c r="B141" s="93" t="s">
@@ -11247,7 +11241,7 @@
       <c r="J141" s="11"/>
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A142" s="156" t="s">
+      <c r="A142" s="153" t="s">
         <v>679</v>
       </c>
       <c r="B142" s="93" t="s">
@@ -11265,7 +11259,7 @@
       <c r="J142" s="11"/>
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A143" s="156" t="s">
+      <c r="A143" s="153" t="s">
         <v>681</v>
       </c>
       <c r="B143" s="93" t="s">
@@ -11283,7 +11277,7 @@
       <c r="J143" s="11"/>
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A144" s="156" t="s">
+      <c r="A144" s="153" t="s">
         <v>684</v>
       </c>
       <c r="B144" s="93" t="s">
@@ -11301,7 +11295,7 @@
       <c r="J144" s="11"/>
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A145" s="156" t="s">
+      <c r="A145" s="153" t="s">
         <v>686</v>
       </c>
       <c r="B145" s="93" t="s">
@@ -11319,7 +11313,7 @@
       <c r="J145" s="11"/>
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A146" s="156" t="s">
+      <c r="A146" s="153" t="s">
         <v>689</v>
       </c>
       <c r="B146" s="93" t="s">
@@ -11337,7 +11331,7 @@
       <c r="J146" s="11"/>
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A147" s="156" t="s">
+      <c r="A147" s="153" t="s">
         <v>691</v>
       </c>
       <c r="B147" s="93" t="s">
@@ -11355,7 +11349,7 @@
       <c r="J147" s="11"/>
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A148" s="156" t="s">
+      <c r="A148" s="153" t="s">
         <v>693</v>
       </c>
       <c r="B148" s="93" t="s">
@@ -11373,7 +11367,7 @@
       <c r="J148" s="11"/>
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A149" s="156" t="s">
+      <c r="A149" s="153" t="s">
         <v>695</v>
       </c>
       <c r="B149" s="93" t="s">
@@ -11391,7 +11385,7 @@
       <c r="J149" s="11"/>
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A150" s="156" t="s">
+      <c r="A150" s="153" t="s">
         <v>697</v>
       </c>
       <c r="B150" s="93" t="s">
@@ -11409,7 +11403,7 @@
       <c r="J150" s="11"/>
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A151" s="156" t="s">
+      <c r="A151" s="153" t="s">
         <v>698</v>
       </c>
       <c r="B151" s="93" t="s">
@@ -11427,7 +11421,7 @@
       <c r="J151" s="11"/>
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A152" s="156" t="s">
+      <c r="A152" s="153" t="s">
         <v>699</v>
       </c>
       <c r="B152" s="93" t="s">
@@ -11445,7 +11439,7 @@
       <c r="J152" s="11"/>
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A153" s="156" t="s">
+      <c r="A153" s="153" t="s">
         <v>701</v>
       </c>
       <c r="B153" s="93" t="s">
@@ -11463,7 +11457,7 @@
       <c r="J153" s="11"/>
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A154" s="156" t="s">
+      <c r="A154" s="153" t="s">
         <v>704</v>
       </c>
       <c r="B154" s="93" t="s">
@@ -11481,7 +11475,7 @@
       <c r="J154" s="11"/>
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A155" s="156" t="s">
+      <c r="A155" s="153" t="s">
         <v>706</v>
       </c>
       <c r="B155" s="93" t="s">
@@ -11499,7 +11493,7 @@
       <c r="J155" s="11"/>
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A156" s="156" t="s">
+      <c r="A156" s="153" t="s">
         <v>709</v>
       </c>
       <c r="B156" s="93" t="s">
@@ -11517,7 +11511,7 @@
       <c r="J156" s="11"/>
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A157" s="156" t="s">
+      <c r="A157" s="153" t="s">
         <v>711</v>
       </c>
       <c r="B157" s="93" t="s">
@@ -11535,7 +11529,7 @@
       <c r="J157" s="11"/>
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A158" s="156" t="s">
+      <c r="A158" s="153" t="s">
         <v>712</v>
       </c>
       <c r="B158" s="93" t="s">
@@ -11553,7 +11547,7 @@
       <c r="J158" s="11"/>
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A159" s="156" t="s">
+      <c r="A159" s="153" t="s">
         <v>714</v>
       </c>
       <c r="B159" s="93" t="s">
@@ -11571,7 +11565,7 @@
       <c r="J159" s="11"/>
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A160" s="156" t="s">
+      <c r="A160" s="153" t="s">
         <v>715</v>
       </c>
       <c r="B160" s="93" t="s">
@@ -11695,8 +11689,8 @@
   </sheetPr>
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:J25"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12055,18 +12049,18 @@
     </row>
     <row r="6" spans="1:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B6" s="11"/>
-      <c r="E6" s="197" t="s">
+      <c r="E6" s="194" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="197"/>
-      <c r="G6" s="197" t="s">
+      <c r="F6" s="194"/>
+      <c r="G6" s="194" t="s">
         <v>67</v>
       </c>
-      <c r="H6" s="197"/>
-      <c r="I6" s="197" t="s">
+      <c r="H6" s="194"/>
+      <c r="I6" s="194" t="s">
         <v>9</v>
       </c>
-      <c r="J6" s="197"/>
+      <c r="J6" s="194"/>
     </row>
     <row r="7" spans="1:11" s="56" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B7" s="11"/>
@@ -12091,18 +12085,18 @@
     </row>
     <row r="8" spans="1:11" s="56" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="11"/>
-      <c r="E8" s="179" t="s">
+      <c r="E8" s="176" t="s">
         <v>200</v>
       </c>
-      <c r="F8" s="179"/>
-      <c r="G8" s="179" t="s">
+      <c r="F8" s="176"/>
+      <c r="G8" s="176" t="s">
         <v>201</v>
       </c>
-      <c r="H8" s="160"/>
-      <c r="I8" s="196" t="s">
+      <c r="H8" s="157"/>
+      <c r="I8" s="193" t="s">
         <v>215</v>
       </c>
-      <c r="J8" s="196"/>
+      <c r="J8" s="193"/>
     </row>
     <row r="9" spans="1:11" s="56" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
       <c r="B9" s="11"/>
@@ -12136,12 +12130,24 @@
       <c r="D10" s="132" t="s">
         <v>175</v>
       </c>
-      <c r="E10" s="141"/>
-      <c r="F10" s="141"/>
-      <c r="G10" s="143"/>
-      <c r="H10" s="143"/>
-      <c r="I10" s="143"/>
-      <c r="J10" s="143"/>
+      <c r="E10" s="141">
+        <v>0</v>
+      </c>
+      <c r="F10" s="141">
+        <v>0</v>
+      </c>
+      <c r="G10" s="196">
+        <v>0</v>
+      </c>
+      <c r="H10" s="196">
+        <v>0</v>
+      </c>
+      <c r="I10" s="196">
+        <v>0</v>
+      </c>
+      <c r="J10" s="196">
+        <v>0</v>
+      </c>
       <c r="K10" s="41"/>
     </row>
     <row r="11" spans="1:11" s="13" customFormat="1" x14ac:dyDescent="0.2">
@@ -12155,12 +12161,24 @@
       <c r="D11" s="133" t="s">
         <v>436</v>
       </c>
-      <c r="E11" s="141"/>
-      <c r="F11" s="141"/>
-      <c r="G11" s="143"/>
-      <c r="H11" s="143"/>
-      <c r="I11" s="143"/>
-      <c r="J11" s="143"/>
+      <c r="E11" s="141">
+        <v>0</v>
+      </c>
+      <c r="F11" s="141">
+        <v>0</v>
+      </c>
+      <c r="G11" s="196">
+        <v>0</v>
+      </c>
+      <c r="H11" s="196">
+        <v>0</v>
+      </c>
+      <c r="I11" s="196">
+        <v>0</v>
+      </c>
+      <c r="J11" s="196">
+        <v>0</v>
+      </c>
       <c r="K11" s="41"/>
     </row>
     <row r="12" spans="1:11" ht="25.5" x14ac:dyDescent="0.2">
@@ -12173,12 +12191,24 @@
       <c r="D12" s="69" t="s">
         <v>437</v>
       </c>
-      <c r="E12" s="142"/>
-      <c r="F12" s="142"/>
-      <c r="G12" s="144"/>
-      <c r="H12" s="144"/>
-      <c r="I12" s="144"/>
-      <c r="J12" s="144"/>
+      <c r="E12" s="141">
+        <v>0</v>
+      </c>
+      <c r="F12" s="141">
+        <v>0</v>
+      </c>
+      <c r="G12" s="196">
+        <v>0</v>
+      </c>
+      <c r="H12" s="196">
+        <v>0</v>
+      </c>
+      <c r="I12" s="196">
+        <v>0</v>
+      </c>
+      <c r="J12" s="196">
+        <v>0</v>
+      </c>
       <c r="K12" s="11"/>
     </row>
     <row r="13" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.2">
@@ -12191,12 +12221,24 @@
       <c r="D13" s="69" t="s">
         <v>438</v>
       </c>
-      <c r="E13" s="142"/>
-      <c r="F13" s="142"/>
-      <c r="G13" s="144"/>
-      <c r="H13" s="144"/>
-      <c r="I13" s="144"/>
-      <c r="J13" s="144"/>
+      <c r="E13" s="141">
+        <v>0</v>
+      </c>
+      <c r="F13" s="141">
+        <v>0</v>
+      </c>
+      <c r="G13" s="196">
+        <v>0</v>
+      </c>
+      <c r="H13" s="196">
+        <v>0</v>
+      </c>
+      <c r="I13" s="196">
+        <v>0</v>
+      </c>
+      <c r="J13" s="196">
+        <v>0</v>
+      </c>
       <c r="K13" s="11"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -12209,12 +12251,24 @@
       <c r="D14" s="69" t="s">
         <v>439</v>
       </c>
-      <c r="E14" s="142"/>
-      <c r="F14" s="142"/>
-      <c r="G14" s="144"/>
-      <c r="H14" s="144"/>
-      <c r="I14" s="144"/>
-      <c r="J14" s="144"/>
+      <c r="E14" s="141">
+        <v>0</v>
+      </c>
+      <c r="F14" s="141">
+        <v>0</v>
+      </c>
+      <c r="G14" s="196">
+        <v>0</v>
+      </c>
+      <c r="H14" s="196">
+        <v>0</v>
+      </c>
+      <c r="I14" s="196">
+        <v>0</v>
+      </c>
+      <c r="J14" s="196">
+        <v>0</v>
+      </c>
       <c r="K14" s="11"/>
     </row>
     <row r="15" spans="1:11" s="13" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12228,12 +12282,24 @@
       <c r="D15" s="69" t="s">
         <v>440</v>
       </c>
-      <c r="E15" s="142"/>
-      <c r="F15" s="142"/>
-      <c r="G15" s="144"/>
-      <c r="H15" s="144"/>
-      <c r="I15" s="144"/>
-      <c r="J15" s="144"/>
+      <c r="E15" s="141">
+        <v>0</v>
+      </c>
+      <c r="F15" s="141">
+        <v>0</v>
+      </c>
+      <c r="G15" s="196">
+        <v>0</v>
+      </c>
+      <c r="H15" s="196">
+        <v>0</v>
+      </c>
+      <c r="I15" s="196">
+        <v>0</v>
+      </c>
+      <c r="J15" s="196">
+        <v>0</v>
+      </c>
       <c r="K15" s="41"/>
     </row>
     <row r="16" spans="1:11" s="34" customFormat="1" ht="43.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12247,12 +12313,24 @@
       <c r="D16" s="133" t="s">
         <v>441</v>
       </c>
-      <c r="E16" s="142"/>
-      <c r="F16" s="142"/>
-      <c r="G16" s="144"/>
-      <c r="H16" s="144"/>
-      <c r="I16" s="144"/>
-      <c r="J16" s="144"/>
+      <c r="E16" s="141">
+        <v>0</v>
+      </c>
+      <c r="F16" s="141">
+        <v>0</v>
+      </c>
+      <c r="G16" s="196">
+        <v>0</v>
+      </c>
+      <c r="H16" s="196">
+        <v>0</v>
+      </c>
+      <c r="I16" s="196">
+        <v>0</v>
+      </c>
+      <c r="J16" s="196">
+        <v>0</v>
+      </c>
       <c r="K16" s="11"/>
     </row>
     <row r="17" spans="1:11" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -12265,12 +12343,24 @@
       <c r="D17" s="69" t="s">
         <v>442</v>
       </c>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
-      <c r="I17" s="144"/>
-      <c r="J17" s="144"/>
+      <c r="E17" s="141">
+        <v>0</v>
+      </c>
+      <c r="F17" s="141">
+        <v>0</v>
+      </c>
+      <c r="G17" s="196">
+        <v>0</v>
+      </c>
+      <c r="H17" s="196">
+        <v>0</v>
+      </c>
+      <c r="I17" s="196">
+        <v>0</v>
+      </c>
+      <c r="J17" s="196">
+        <v>0</v>
+      </c>
       <c r="K17" s="11"/>
     </row>
     <row r="18" spans="1:11" s="20" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12284,12 +12374,24 @@
       <c r="D18" s="69" t="s">
         <v>439</v>
       </c>
-      <c r="E18" s="142"/>
-      <c r="F18" s="142"/>
-      <c r="G18" s="144"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="144"/>
-      <c r="J18" s="144"/>
+      <c r="E18" s="141">
+        <v>0</v>
+      </c>
+      <c r="F18" s="141">
+        <v>0</v>
+      </c>
+      <c r="G18" s="196">
+        <v>0</v>
+      </c>
+      <c r="H18" s="196">
+        <v>0</v>
+      </c>
+      <c r="I18" s="196">
+        <v>0</v>
+      </c>
+      <c r="J18" s="196">
+        <v>0</v>
+      </c>
       <c r="K18" s="11"/>
     </row>
     <row r="19" spans="1:11" s="34" customFormat="1" x14ac:dyDescent="0.2">
@@ -12303,12 +12405,24 @@
       <c r="D19" s="69" t="s">
         <v>440</v>
       </c>
-      <c r="E19" s="142"/>
-      <c r="F19" s="142"/>
-      <c r="G19" s="144"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="144"/>
-      <c r="J19" s="144"/>
+      <c r="E19" s="141">
+        <v>0</v>
+      </c>
+      <c r="F19" s="141">
+        <v>0</v>
+      </c>
+      <c r="G19" s="196">
+        <v>0</v>
+      </c>
+      <c r="H19" s="196">
+        <v>0</v>
+      </c>
+      <c r="I19" s="196">
+        <v>0</v>
+      </c>
+      <c r="J19" s="196">
+        <v>0</v>
+      </c>
       <c r="K19" s="11"/>
     </row>
     <row r="20" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -12321,12 +12435,24 @@
       <c r="D20" s="133" t="s">
         <v>443</v>
       </c>
-      <c r="E20" s="142"/>
-      <c r="F20" s="142"/>
-      <c r="G20" s="144"/>
-      <c r="H20" s="144"/>
-      <c r="I20" s="144"/>
-      <c r="J20" s="144"/>
+      <c r="E20" s="141">
+        <v>0</v>
+      </c>
+      <c r="F20" s="141">
+        <v>0</v>
+      </c>
+      <c r="G20" s="196">
+        <v>0</v>
+      </c>
+      <c r="H20" s="196">
+        <v>0</v>
+      </c>
+      <c r="I20" s="196">
+        <v>0</v>
+      </c>
+      <c r="J20" s="196">
+        <v>0</v>
+      </c>
       <c r="K20" s="11"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -12339,12 +12465,24 @@
       <c r="D21" s="132" t="s">
         <v>177</v>
       </c>
-      <c r="E21" s="142"/>
-      <c r="F21" s="142"/>
-      <c r="G21" s="144"/>
-      <c r="H21" s="144"/>
-      <c r="I21" s="144"/>
-      <c r="J21" s="144"/>
+      <c r="E21" s="141">
+        <v>0</v>
+      </c>
+      <c r="F21" s="141">
+        <v>0</v>
+      </c>
+      <c r="G21" s="196">
+        <v>0</v>
+      </c>
+      <c r="H21" s="196">
+        <v>0</v>
+      </c>
+      <c r="I21" s="196">
+        <v>0</v>
+      </c>
+      <c r="J21" s="196">
+        <v>0</v>
+      </c>
       <c r="K21" s="11"/>
     </row>
     <row r="22" spans="1:11" ht="34.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12357,12 +12495,24 @@
       <c r="D22" s="108" t="s">
         <v>444</v>
       </c>
-      <c r="E22" s="142"/>
-      <c r="F22" s="142"/>
-      <c r="G22" s="144"/>
-      <c r="H22" s="144"/>
-      <c r="I22" s="144"/>
-      <c r="J22" s="144"/>
+      <c r="E22" s="141">
+        <v>0</v>
+      </c>
+      <c r="F22" s="141">
+        <v>0</v>
+      </c>
+      <c r="G22" s="196">
+        <v>0</v>
+      </c>
+      <c r="H22" s="196">
+        <v>0</v>
+      </c>
+      <c r="I22" s="196">
+        <v>0</v>
+      </c>
+      <c r="J22" s="196">
+        <v>0</v>
+      </c>
       <c r="K22" s="11"/>
     </row>
     <row r="23" spans="1:11" s="34" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
@@ -12376,12 +12526,24 @@
       <c r="D23" s="108" t="s">
         <v>445</v>
       </c>
-      <c r="E23" s="142"/>
-      <c r="F23" s="142"/>
-      <c r="G23" s="144"/>
-      <c r="H23" s="144"/>
-      <c r="I23" s="144"/>
-      <c r="J23" s="144"/>
+      <c r="E23" s="141">
+        <v>0</v>
+      </c>
+      <c r="F23" s="141">
+        <v>0</v>
+      </c>
+      <c r="G23" s="196">
+        <v>0</v>
+      </c>
+      <c r="H23" s="196">
+        <v>0</v>
+      </c>
+      <c r="I23" s="196">
+        <v>0</v>
+      </c>
+      <c r="J23" s="196">
+        <v>0</v>
+      </c>
       <c r="K23" s="11"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -12394,12 +12556,24 @@
       <c r="D24" s="82" t="s">
         <v>443</v>
       </c>
-      <c r="E24" s="142"/>
-      <c r="F24" s="142"/>
-      <c r="G24" s="144"/>
-      <c r="H24" s="144"/>
-      <c r="I24" s="144"/>
-      <c r="J24" s="144"/>
+      <c r="E24" s="141">
+        <v>0</v>
+      </c>
+      <c r="F24" s="141">
+        <v>0</v>
+      </c>
+      <c r="G24" s="196">
+        <v>0</v>
+      </c>
+      <c r="H24" s="196">
+        <v>0</v>
+      </c>
+      <c r="I24" s="196">
+        <v>0</v>
+      </c>
+      <c r="J24" s="196">
+        <v>0</v>
+      </c>
       <c r="K24" s="11"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -12569,7 +12743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A4:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G29" sqref="G29:G30"/>
     </sheetView>
   </sheetViews>
@@ -12612,104 +12786,104 @@
       <c r="G6" s="34"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="145"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="198" t="s">
+      <c r="A7" s="142"/>
+      <c r="B7" s="143"/>
+      <c r="C7" s="195" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="198"/>
-      <c r="E7" s="198"/>
-      <c r="F7" s="198"/>
-      <c r="G7" s="198"/>
-      <c r="H7" s="198"/>
-      <c r="I7" s="198"/>
+      <c r="D7" s="195"/>
+      <c r="E7" s="195"/>
+      <c r="F7" s="195"/>
+      <c r="G7" s="195"/>
+      <c r="H7" s="195"/>
+      <c r="I7" s="195"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="147" t="s">
+      <c r="A8" s="144" t="s">
         <v>70</v>
       </c>
-      <c r="B8" s="147"/>
-      <c r="C8" s="148" t="s">
+      <c r="B8" s="144"/>
+      <c r="C8" s="145" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="148" t="s">
+      <c r="D8" s="145" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="148" t="s">
+      <c r="E8" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="148" t="s">
+      <c r="F8" s="145" t="s">
         <v>4</v>
       </c>
-      <c r="G8" s="148" t="s">
+      <c r="G8" s="145" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="148" t="s">
+      <c r="H8" s="145" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="148" t="s">
+      <c r="I8" s="145" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="149" t="s">
+      <c r="A9" s="146" t="s">
         <v>455</v>
       </c>
-      <c r="B9" s="150" t="s">
+      <c r="B9" s="147" t="s">
         <v>456</v>
       </c>
-      <c r="C9" s="152"/>
-      <c r="D9" s="152"/>
-      <c r="E9" s="152"/>
-      <c r="F9" s="152"/>
-      <c r="G9" s="152"/>
-      <c r="H9" s="152"/>
-      <c r="I9" s="152"/>
+      <c r="C9" s="149"/>
+      <c r="D9" s="149"/>
+      <c r="E9" s="149"/>
+      <c r="F9" s="149"/>
+      <c r="G9" s="149"/>
+      <c r="H9" s="149"/>
+      <c r="I9" s="149"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="149" t="s">
+      <c r="A10" s="146" t="s">
         <v>457</v>
       </c>
-      <c r="B10" s="150" t="s">
+      <c r="B10" s="147" t="s">
         <v>458</v>
       </c>
-      <c r="C10" s="152"/>
-      <c r="D10" s="152"/>
-      <c r="E10" s="152"/>
-      <c r="F10" s="152"/>
-      <c r="G10" s="152"/>
-      <c r="H10" s="152"/>
-      <c r="I10" s="152"/>
+      <c r="C10" s="149"/>
+      <c r="D10" s="149"/>
+      <c r="E10" s="149"/>
+      <c r="F10" s="149"/>
+      <c r="G10" s="149"/>
+      <c r="H10" s="149"/>
+      <c r="I10" s="149"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="149" t="s">
+      <c r="A11" s="146" t="s">
         <v>459</v>
       </c>
-      <c r="B11" s="150" t="s">
+      <c r="B11" s="147" t="s">
         <v>460</v>
       </c>
-      <c r="C11" s="152"/>
-      <c r="D11" s="152"/>
-      <c r="E11" s="152"/>
-      <c r="F11" s="152"/>
-      <c r="G11" s="152"/>
-      <c r="H11" s="152"/>
-      <c r="I11" s="152"/>
+      <c r="C11" s="149"/>
+      <c r="D11" s="149"/>
+      <c r="E11" s="149"/>
+      <c r="F11" s="149"/>
+      <c r="G11" s="149"/>
+      <c r="H11" s="149"/>
+      <c r="I11" s="149"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="149" t="s">
+      <c r="A12" s="146" t="s">
         <v>218</v>
       </c>
-      <c r="B12" s="150" t="s">
+      <c r="B12" s="147" t="s">
         <v>461</v>
       </c>
-      <c r="C12" s="151"/>
-      <c r="D12" s="151"/>
-      <c r="E12" s="151"/>
-      <c r="F12" s="151"/>
-      <c r="G12" s="151"/>
-      <c r="H12" s="151"/>
-      <c r="I12" s="151"/>
+      <c r="C12" s="148"/>
+      <c r="D12" s="148"/>
+      <c r="E12" s="148"/>
+      <c r="F12" s="148"/>
+      <c r="G12" s="148"/>
+      <c r="H12" s="148"/>
+      <c r="I12" s="148"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="34"/>

</xml_diff>